<commit_message>
more fully implemented dashboard with game preview
</commit_message>
<xml_diff>
--- a/csv/csv_test1.xlsx
+++ b/csv/csv_test1.xlsx
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Question</t>
   </si>
   <si>
-    <t>Correct</t>
-  </si>
-  <si>
     <t>What is not a color</t>
   </si>
   <si>
@@ -73,6 +70,30 @@
   </si>
   <si>
     <t>Guava</t>
+  </si>
+  <si>
+    <t>Correct Answer</t>
+  </si>
+  <si>
+    <t>Wrong Answer 1</t>
+  </si>
+  <si>
+    <t>Wrong Answer 2</t>
+  </si>
+  <si>
+    <t>Wrong Answer 3</t>
+  </si>
+  <si>
+    <t>Wrong Answer 4</t>
+  </si>
+  <si>
+    <t>Wrong Answer 5</t>
+  </si>
+  <si>
+    <t>Wrong Answer 6</t>
+  </si>
+  <si>
+    <t>Wrong Answer 7</t>
   </si>
 </sst>
 </file>
@@ -453,7 +474,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -467,29 +488,50 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -500,36 +542,36 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
       <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>4</v>

</xml_diff>